<commit_message>
Modificacion de subir archivo de excel
</commit_message>
<xml_diff>
--- a/GestionOrdenamientos/Documentos/subirCiklos.xlsx
+++ b/GestionOrdenamientos/Documentos/subirCiklos.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LUISM\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15312" windowHeight="7704"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15315" windowHeight="7710"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -128,9 +128,6 @@
     <t>FechaActualizoProveedor</t>
   </si>
   <si>
-    <t>LUISA FERNANDA RAMIREZ GRANADA ( E D )</t>
-  </si>
-  <si>
     <t>EN ESTUDIO</t>
   </si>
   <si>
@@ -225,6 +222,9 @@
   </si>
   <si>
     <t>TI - 1036634597</t>
+  </si>
+  <si>
+    <t>aaa</t>
   </si>
 </sst>
 </file>
@@ -561,47 +561,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AH1" sqref="AH1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -705,7 +704,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>172899089</v>
       </c>
@@ -713,60 +712,60 @@
         <v>42830</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="D2" s="2">
         <v>42830</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="S2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T2" s="1"/>
       <c r="U2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Y2" s="1">
         <v>452301</v>
@@ -781,7 +780,7 @@
       <c r="AG2" s="1"/>
       <c r="AH2" s="1"/>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>172912866</v>
       </c>
@@ -789,60 +788,60 @@
         <v>42830</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" s="2">
         <v>42830</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R3" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="S3" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T3" s="1"/>
       <c r="U3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
       <c r="X3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Y3" s="1">
         <v>452301</v>
@@ -857,7 +856,7 @@
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>172947889</v>
       </c>
@@ -865,56 +864,56 @@
         <v>42830</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" s="2">
         <v>42830</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="R4" s="1"/>
       <c r="S4" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Y4" s="1">
         <v>907106</v>
@@ -929,7 +928,7 @@
       <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>173141113</v>
       </c>
@@ -937,58 +936,58 @@
         <v>42830</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5" s="2">
         <v>42830</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="M5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="O5" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="P5" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="Q5" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R5" s="1"/>
       <c r="S5" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
       <c r="W5" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Y5" s="1">
         <v>890394</v>

</xml_diff>